<commit_message>
Updated parsing of CPR Stockpile
</commit_message>
<xml_diff>
--- a/docs/Manual Input Template.xlsx
+++ b/docs/Manual Input Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\em-dashboard-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\em-dashboard-parser\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2511BE8F-76D8-40A0-97B1-51BF9A764DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47854A2D-BB6B-4C03-8789-79593C99D4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{844CFE0B-F18F-4AEF-86D4-A245206B668E}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{844CFE0B-F18F-4AEF-86D4-A245206B668E}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Qinhuangdao</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>CCI 4700</t>
+  </si>
+  <si>
+    <t>Huadian Caofeidian</t>
   </si>
 </sst>
 </file>
@@ -203,19 +206,21 @@
     <xf numFmtId="4" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,10 +544,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="9"/>
-    <col min="2" max="4" width="20.7109375" style="10"/>
-    <col min="5" max="5" width="20.7109375" style="11"/>
-    <col min="6" max="16384" width="20.7109375" style="8"/>
+    <col min="1" max="1" width="20.7109375" style="8"/>
+    <col min="2" max="4" width="20.7109375" style="9"/>
+    <col min="5" max="5" width="20.7109375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -581,21 +585,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F30DD6-A2F0-447D-8147-9499E2BEF23C}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="9"/>
-    <col min="2" max="10" width="20.7109375" style="12"/>
-    <col min="11" max="11" width="20.7109375" style="11"/>
-    <col min="12" max="16384" width="20.7109375" style="8"/>
+    <col min="1" max="1" width="20.7109375" style="8"/>
+    <col min="2" max="11" width="20.7109375" style="11"/>
+    <col min="12" max="12" width="20.7109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -620,13 +623,16 @@
       <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -635,15 +641,16 @@
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{6BAB8138-37D4-4BAF-8DF6-0B81F7FF53CD}">
       <formula1>43831</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{4B083FA2-F4D2-481C-AF18-B1D0020FC2C4}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{4B083FA2-F4D2-481C-AF18-B1D0020FC2C4}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:J1048576" xr:uid="{B74A7B7F-5920-4527-A2D7-D01F74AA9F32}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:K1048576" xr:uid="{B74A7B7F-5920-4527-A2D7-D01F74AA9F32}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -657,11 +664,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="9"/>
-    <col min="2" max="4" width="20.7109375" style="10"/>
-    <col min="5" max="5" width="20.7109375" style="12"/>
-    <col min="6" max="6" width="20.7109375" style="11"/>
-    <col min="7" max="16384" width="20.7109375" style="8"/>
+    <col min="1" max="1" width="20.7109375" style="8"/>
+    <col min="2" max="4" width="20.7109375" style="9"/>
+    <col min="5" max="5" width="20.7109375" style="11"/>
+    <col min="6" max="6" width="20.7109375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -712,10 +718,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="9"/>
-    <col min="2" max="3" width="20.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="20.7109375" style="8"/>
+    <col min="1" max="1" width="20.7109375" style="8"/>
+    <col min="2" max="3" width="20.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -733,10 +738,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -759,16 +764,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCA86FA-344F-4F96-8757-F088ECF29D60}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="9"/>
-    <col min="2" max="5" width="20.7109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="20.7109375" style="8"/>
+    <col min="1" max="1" width="20.7109375" style="8"/>
+    <col min="2" max="5" width="20.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Completed Russian rail coal export fact parsing
</commit_message>
<xml_diff>
--- a/docs/Manual Input Template.xlsx
+++ b/docs/Manual Input Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\em-dashboard-parser\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Skrine\Desktop\Code\Sakhalin\prod\em-dashboard-parser\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47854A2D-BB6B-4C03-8789-79593C99D4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C62346-3B23-4CDC-8C00-CAB6477C8C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{844CFE0B-F18F-4AEF-86D4-A245206B668E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{844CFE0B-F18F-4AEF-86D4-A245206B668E}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Freight" sheetId="2" r:id="rId3"/>
     <sheet name="Futures" sheetId="4" r:id="rId4"/>
     <sheet name="China Weather" sheetId="5" r:id="rId5"/>
+    <sheet name="Coal Rail Exports" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Qinhuangdao</t>
   </si>
@@ -112,6 +113,15 @@
   </si>
   <si>
     <t>Huadian Caofeidian</t>
+  </si>
+  <si>
+    <t>Southern Volume</t>
+  </si>
+  <si>
+    <t>Eastern Volume</t>
+  </si>
+  <si>
+    <t>Northwestern Volume</t>
   </si>
 </sst>
 </file>
@@ -542,14 +552,14 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="8"/>
-    <col min="2" max="4" width="20.7109375" style="9"/>
-    <col min="5" max="5" width="20.7109375" style="10"/>
+    <col min="1" max="1" width="20.6640625" style="8"/>
+    <col min="2" max="4" width="20.6640625" style="9"/>
+    <col min="5" max="5" width="20.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -587,18 +597,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F30DD6-A2F0-447D-8147-9499E2BEF23C}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="8"/>
-    <col min="2" max="11" width="20.7109375" style="11"/>
-    <col min="12" max="12" width="20.7109375" style="10"/>
+    <col min="1" max="1" width="20.6640625" style="8"/>
+    <col min="2" max="11" width="20.6640625" style="11"/>
+    <col min="12" max="12" width="20.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -662,15 +672,15 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="8"/>
-    <col min="2" max="4" width="20.7109375" style="9"/>
-    <col min="5" max="5" width="20.7109375" style="11"/>
-    <col min="6" max="6" width="20.7109375" style="10"/>
+    <col min="1" max="1" width="20.6640625" style="8"/>
+    <col min="2" max="4" width="20.6640625" style="9"/>
+    <col min="5" max="5" width="20.6640625" style="11"/>
+    <col min="6" max="6" width="20.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -716,14 +726,14 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="8"/>
-    <col min="2" max="3" width="20.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="8"/>
+    <col min="2" max="3" width="20.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -737,7 +747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -765,17 +775,17 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="8"/>
-    <col min="2" max="5" width="20.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="8"/>
+    <col min="2" max="5" width="20.6640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -810,4 +820,54 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5C5584-7470-44D6-B68E-E33F1433554A}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" style="8"/>
+    <col min="2" max="5" width="20.6640625" style="11"/>
+    <col min="6" max="6" width="20.6640625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:D1048576 E2:E1048576" xr:uid="{AFC71C83-D70E-4C0F-9031-971272306788}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{ABABCA0D-1D6C-49BA-8A84-49F78AB9A97E}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:XFD1048576" xr:uid="{36FD744C-7BB1-44C6-BA52-105017B3435E}"/>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{EBA66172-6F0C-4096-9D14-5603D0CCE478}">
+      <formula1>43831</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>